<commit_message>
Modified functions: Repeat_features and adding ReadDefs_ProdFreq
</commit_message>
<xml_diff>
--- a/Correlation Summary.xlsx
+++ b/Correlation Summary.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d4eb0f181e38d40/PhD/VSA_Concepts_Weighted/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jobqu\OneDrive\PhD\VSA_MEN_concepts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="455" documentId="8_{142A3348-7B62-4F84-A9B8-CA7D0843BEB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{769A291D-EA2E-47C0-9776-B37B943BDB95}"/>
+  <xr:revisionPtr revIDLastSave="549" documentId="8_{142A3348-7B62-4F84-A9B8-CA7D0843BEB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2DEE8135-9902-487D-AD5F-3B8BAA06E0A9}"/>
   <bookViews>
     <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{AA7D028F-3842-4D8E-9E4C-60C088FCA9FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="SOLO MEN" sheetId="2" r:id="rId1"/>
+    <sheet name="Anterior" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Mi dataset (64)</t>
   </si>
@@ -148,13 +149,58 @@
   </si>
   <si>
     <t>conceptos de MEN</t>
+  </si>
+  <si>
+    <t>HDC ('normal', 30, MEN_names)</t>
+  </si>
+  <si>
+    <t>BUSCAR MÁS MÉTODOS… que pueda correr personalmente</t>
+  </si>
+  <si>
+    <t>HDC ('Prod_Freq', 7, MEN)</t>
+  </si>
+  <si>
+    <t>HDC ('Prod_Freq', 15, MEN)</t>
+  </si>
+  <si>
+    <t>HDC ('Prod_Freq', 23, MEN)</t>
+  </si>
+  <si>
+    <t>[7, 11, 16]</t>
+  </si>
+  <si>
+    <t>[11, 16, 21]</t>
+  </si>
+  <si>
+    <t>HDC ('Prod_Freq', 30, MEN)</t>
+  </si>
+  <si>
+    <t>[14, 18, 22]</t>
+  </si>
+  <si>
+    <t>[17, 21, 23]</t>
+  </si>
+  <si>
+    <t>[18, 22, 25]</t>
+  </si>
+  <si>
+    <t>[12, 16, 18]</t>
+  </si>
+  <si>
+    <t>[7,8,9]</t>
+  </si>
+  <si>
+    <t>[7,8,10]</t>
+  </si>
+  <si>
+    <t>[7,8,11]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +224,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +256,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -217,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,9 +316,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -260,6 +327,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,11 +709,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761BBAD2-2891-4E6D-849E-CEB918A1F823}">
+  <dimension ref="B4:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7">
+        <f>AVERAGE(0.6727,0.672738)</f>
+        <v>0.67271899999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4">
+        <f>AVERAGE(0.6634,0.67401)</f>
+        <v>0.66870499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4">
+        <f>AVERAGE(0.5844,5844)</f>
+        <v>2922.2921999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.57750000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.31719999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.61865999999999999</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.63160000000000005</v>
+      </c>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.63929999999999998</v>
+      </c>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.62629999999999997</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.64429999999999998</v>
+      </c>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.64558000000000004</v>
+      </c>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.65820000000000001</v>
+      </c>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.66624000000000005</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="20">
+        <f>AVERAGE(0.6754,0.6537, 0.6692, 0.666)</f>
+        <v>0.66607499999999997</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.66339999999999999</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.65669999999999995</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:C10">
+    <sortCondition descending="1" ref="C10"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D16:D19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F04EE2-E08C-4134-A350-CA3B8CC9EC3F}">
   <dimension ref="E6:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="E6:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -640,10 +942,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="5" t="s">
         <v>1</v>
       </c>
@@ -950,7 +1252,7 @@
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="14">
+      <c r="L20" s="13">
         <v>0.65429999999999999</v>
       </c>
     </row>
@@ -970,12 +1272,12 @@
         <v>0.66600000000000004</v>
       </c>
       <c r="K21" s="8"/>
-      <c r="L21" s="14">
+      <c r="L21" s="13">
         <v>0.66520000000000001</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="4">
@@ -996,12 +1298,12 @@
       <c r="K22" s="4">
         <v>0.50870000000000004</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="11">
         <v>0.52029999999999998</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="4">
@@ -1022,12 +1324,12 @@
       <c r="K23" s="4">
         <v>0.50209999999999999</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="11">
         <v>0.505</v>
       </c>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="4">
@@ -1048,12 +1350,12 @@
       <c r="K24" s="4">
         <v>0.53690000000000004</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="11">
         <v>0.53310000000000002</v>
       </c>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="4">
@@ -1074,7 +1376,7 @@
       <c r="K25" s="4">
         <v>0.53879999999999995</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="11">
         <v>0.53910000000000002</v>
       </c>
       <c r="M25" t="s">
@@ -1082,7 +1384,7 @@
       </c>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>15</v>
       </c>
       <c r="F26" s="4">
@@ -1101,18 +1403,18 @@
       <c r="K26" s="4">
         <v>0.58640000000000003</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="11">
         <v>0.5736</v>
       </c>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <v>20</v>
       </c>
       <c r="F27" s="4">
         <v>0.67290000000000005</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="12">
         <v>0.69240000000000002</v>
       </c>
       <c r="H27" s="4">
@@ -1125,65 +1427,65 @@
       <c r="K27" s="4">
         <v>0.57850000000000001</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="11">
         <v>0.57989999999999997</v>
       </c>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E28" s="11">
+      <c r="E28" s="10">
         <v>30</v>
       </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11">
         <v>0.67764999999999997</v>
       </c>
-      <c r="H28" s="12"/>
-      <c r="I28" s="14">
+      <c r="H28" s="11"/>
+      <c r="I28" s="13">
         <v>0.64100000000000001</v>
       </c>
-      <c r="J28" s="12"/>
+      <c r="J28" s="11"/>
       <c r="K28" s="4">
         <v>0.59</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="11">
         <v>0.58670999999999995</v>
       </c>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>50</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11">
+      <c r="F29" s="11"/>
+      <c r="G29" s="10">
         <v>0.68659999999999999</v>
       </c>
-      <c r="H29" s="12"/>
-      <c r="I29" s="14">
+      <c r="H29" s="11"/>
+      <c r="I29" s="13">
         <v>0.6502</v>
       </c>
-      <c r="J29" s="12"/>
+      <c r="J29" s="11"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="12">
+      <c r="L29" s="11">
         <v>0.58130000000000004</v>
       </c>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E30" s="11">
+      <c r="E30" s="10">
         <v>100</v>
       </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11">
+      <c r="F30" s="11"/>
+      <c r="G30" s="10">
         <v>0.68589999999999995</v>
       </c>
-      <c r="H30" s="12"/>
-      <c r="I30" s="14">
+      <c r="H30" s="11"/>
+      <c r="I30" s="13">
         <v>0.64400000000000002</v>
       </c>
-      <c r="J30" s="12"/>
+      <c r="J30" s="11"/>
       <c r="K30" s="4">
         <v>0.59</v>
       </c>
-      <c r="L30" s="12">
+      <c r="L30" s="11">
         <v>0.57589999999999997</v>
       </c>
     </row>
@@ -1410,19 +1712,19 @@
       </c>
     </row>
     <row r="40" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="4">
         <v>0.53959999999999997</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="11">
         <v>0.53320000000000001</v>
       </c>
       <c r="H40" s="4">
         <v>0.50800000000000001</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="11">
         <v>0.50349999999999995</v>
       </c>
       <c r="J40" s="4">
@@ -1431,24 +1733,24 @@
       <c r="K40" s="4">
         <v>0.44069999999999998</v>
       </c>
-      <c r="L40" s="12">
+      <c r="L40" s="11">
         <v>0.432</v>
       </c>
     </row>
     <row r="41" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F41" s="4">
         <v>0.58411000000000002</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="11">
         <v>0.56610000000000005</v>
       </c>
       <c r="H41" s="4">
         <v>0.53649999999999998</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41" s="11">
         <v>0.53159999999999996</v>
       </c>
       <c r="J41" s="4">
@@ -1457,161 +1759,161 @@
       <c r="K41" s="4">
         <v>0.45639999999999997</v>
       </c>
-      <c r="L41" s="12">
+      <c r="L41" s="11">
         <v>0.46839999999999998</v>
       </c>
     </row>
     <row r="42" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F42" s="4">
         <v>0.57125000000000004</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="11">
         <v>0.58099999999999996</v>
       </c>
       <c r="H42" s="4">
         <v>0.57540000000000002</v>
       </c>
-      <c r="I42" s="12">
+      <c r="I42" s="11">
         <v>0.57279999999999998</v>
       </c>
-      <c r="J42" s="12"/>
+      <c r="J42" s="11"/>
       <c r="K42" s="4">
         <v>0.46239999999999998</v>
       </c>
-      <c r="L42" s="12">
+      <c r="L42" s="11">
         <v>0.46100000000000002</v>
       </c>
     </row>
     <row r="43" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F43" s="4">
         <v>0.5968</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="11">
         <v>0.58589999999999998</v>
       </c>
       <c r="H43" s="4">
         <v>0.5827</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I43" s="11">
         <v>0.56789999999999996</v>
       </c>
-      <c r="J43" s="12"/>
+      <c r="J43" s="11"/>
       <c r="K43" s="4">
         <v>0.44969999999999999</v>
       </c>
-      <c r="L43" s="12">
+      <c r="L43" s="11">
         <v>0.45400000000000001</v>
       </c>
     </row>
     <row r="44" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E44" s="11">
+      <c r="E44" s="10">
         <v>15</v>
       </c>
       <c r="F44" s="4">
         <v>0.58550000000000002</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="11">
         <v>0.59370000000000001</v>
       </c>
       <c r="H44" s="4">
         <v>0.57969999999999999</v>
       </c>
-      <c r="I44" s="12">
+      <c r="I44" s="11">
         <v>0.57550000000000001</v>
       </c>
-      <c r="J44" s="12"/>
+      <c r="J44" s="11"/>
       <c r="K44" s="4">
         <v>0.45200000000000001</v>
       </c>
-      <c r="L44" s="12">
+      <c r="L44" s="11">
         <v>0.46760000000000002</v>
       </c>
     </row>
     <row r="45" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E45" s="11">
+      <c r="E45" s="10">
         <v>20</v>
       </c>
       <c r="F45" s="4">
         <v>0.58860000000000001</v>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="11">
         <v>0.58330000000000004</v>
       </c>
       <c r="H45" s="4">
         <v>0.56689999999999996</v>
       </c>
-      <c r="I45" s="12">
+      <c r="I45" s="11">
         <v>0.58316000000000001</v>
       </c>
-      <c r="J45" s="12"/>
+      <c r="J45" s="11"/>
       <c r="K45" s="4">
         <v>0.4743</v>
       </c>
-      <c r="L45" s="12">
+      <c r="L45" s="11">
         <v>0.46610000000000001</v>
       </c>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E46" s="11">
+      <c r="E46" s="10">
         <v>30</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="12">
+      <c r="G46" s="11">
         <v>0.59289999999999998</v>
       </c>
       <c r="H46" s="4"/>
-      <c r="I46" s="12">
+      <c r="I46" s="11">
         <v>0.58479999999999999</v>
       </c>
-      <c r="J46" s="12"/>
+      <c r="J46" s="11"/>
       <c r="K46" s="4">
         <v>0.46250000000000002</v>
       </c>
-      <c r="L46" s="12">
+      <c r="L46" s="11">
         <v>0.46589999999999998</v>
       </c>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E47" s="11">
+      <c r="E47" s="10">
         <v>50</v>
       </c>
       <c r="F47" s="4"/>
-      <c r="G47" s="12">
+      <c r="G47" s="11">
         <v>0.59440000000000004</v>
       </c>
       <c r="H47" s="4"/>
-      <c r="I47" s="12">
+      <c r="I47" s="11">
         <v>0.58160000000000001</v>
       </c>
-      <c r="J47" s="12"/>
+      <c r="J47" s="11"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="12">
+      <c r="L47" s="11">
         <v>0.46250000000000002</v>
       </c>
     </row>
     <row r="48" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E48" s="11">
+      <c r="E48" s="10">
         <v>100</v>
       </c>
       <c r="F48" s="4"/>
-      <c r="G48" s="12">
+      <c r="G48" s="11">
         <v>0.57840000000000003</v>
       </c>
       <c r="H48" s="4"/>
-      <c r="I48" s="12">
+      <c r="I48" s="11">
         <v>0.59140000000000004</v>
       </c>
-      <c r="J48" s="12"/>
+      <c r="J48" s="11"/>
       <c r="K48" s="4">
         <v>0.45889999999999997</v>
       </c>
-      <c r="L48" s="12">
+      <c r="L48" s="11">
         <v>0.46600000000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some data exploration of the MEN's concepts within the McRae dataset. I added the function Weight_Features in EncodingDataset notebook.
</commit_message>
<xml_diff>
--- a/Correlation Summary.xlsx
+++ b/Correlation Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jobqu\OneDrive\PhD\VSA_MEN_concepts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d4eb0f181e38d40/PhD/VSA_MEN_concepts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="8_{142A3348-7B62-4F84-A9B8-CA7D0843BEB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2DEE8135-9902-487D-AD5F-3B8BAA06E0A9}"/>
+  <xr:revisionPtr revIDLastSave="595" documentId="8_{142A3348-7B62-4F84-A9B8-CA7D0843BEB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{20B9CA29-728F-4385-8EBF-97C596A461AA}"/>
   <bookViews>
     <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{AA7D028F-3842-4D8E-9E4C-60C088FCA9FA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Mi dataset (64)</t>
   </si>
@@ -187,13 +187,22 @@
     <t>[12, 16, 18]</t>
   </si>
   <si>
-    <t>[7,8,9]</t>
-  </si>
-  <si>
-    <t>[7,8,10]</t>
-  </si>
-  <si>
-    <t>[7,8,11]</t>
+    <t>CAMBIO DE MÉTODO… AHORA PESAMOS CADA FEATURE CON BASE EN PROD_FREQ</t>
+  </si>
+  <si>
+    <t>Método 5 divisiones…</t>
+  </si>
+  <si>
+    <t>Método 4 divisiones…</t>
+  </si>
+  <si>
+    <t>Método 3 divisiones…</t>
+  </si>
+  <si>
+    <t>Método 2 divisiones…</t>
+  </si>
+  <si>
+    <t>Método 6 divisiones…</t>
   </si>
 </sst>
 </file>
@@ -287,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,12 +337,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,11 +353,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761BBAD2-2891-4E6D-849E-CEB918A1F823}">
-  <dimension ref="B4:D34"/>
+  <dimension ref="B4:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -722,12 +734,15 @@
     <col min="3" max="3" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
@@ -736,7 +751,7 @@
         <v>0.67271899999999996</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>39</v>
       </c>
@@ -745,7 +760,7 @@
         <v>0.66870499999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -754,7 +769,7 @@
         <v>2922.2921999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -762,162 +777,234 @@
         <v>0.57750000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4">
         <v>0.55700000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
         <v>0.31719999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="G10" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="4">
+        <v>0.64239999999999997</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.63890000000000002</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.64319999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="4">
         <v>0.61865999999999999</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="4">
         <v>0.63160000000000005</v>
       </c>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="18"/>
+      <c r="G13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="4">
+        <v>0.65229999999999999</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.65459999999999996</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.64480000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="12">
         <v>0.63929999999999998</v>
       </c>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="4">
         <v>0.62629999999999997</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="4">
+        <v>0.65259999999999996</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.65649999999999997</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.65739999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="4">
         <v>0.64429999999999998</v>
       </c>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="4">
         <v>0.64558000000000004</v>
       </c>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="19"/>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="12">
         <v>0.65820000000000001</v>
       </c>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="19"/>
+      <c r="G19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="4">
+        <v>0.6552</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.65800999999999998</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.66739999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="4">
         <v>0.66624000000000005</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G22" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="4">
+        <v>0.66439999999999999</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="17">
         <f>AVERAGE(0.6754,0.6537, 0.6692, 0.666)</f>
         <v>0.66607499999999997</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="4">
         <v>0.66339999999999999</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="4">
         <v>0.65669999999999995</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="16" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:C10">
     <sortCondition descending="1" ref="C10"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D16:D19"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -942,10 +1029,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Finished some test. The best to encode (so far) is by only considering Interr_str_tax...
</commit_message>
<xml_diff>
--- a/Correlation Summary.xlsx
+++ b/Correlation Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d4eb0f181e38d40/PhD/VSA_MEN_concepts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jobqu\OneDrive\PhD\VSA_MEN_concepts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="595" documentId="8_{142A3348-7B62-4F84-A9B8-CA7D0843BEB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{20B9CA29-728F-4385-8EBF-97C596A461AA}"/>
+  <xr:revisionPtr revIDLastSave="697" documentId="8_{142A3348-7B62-4F84-A9B8-CA7D0843BEB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0A1611F2-E8AF-4BA8-B843-1DF83D5E5ACE}"/>
   <bookViews>
     <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{AA7D028F-3842-4D8E-9E4C-60C088FCA9FA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>Mi dataset (64)</t>
   </si>
@@ -203,6 +203,51 @@
   </si>
   <si>
     <t>Método 6 divisiones…</t>
+  </si>
+  <si>
+    <t>CON Intercorr_str_tax…</t>
+  </si>
+  <si>
+    <t>HDC ('Intercorr_str_tax', 30, MEN)</t>
+  </si>
+  <si>
+    <t>Método con 2 divisiones…</t>
+  </si>
+  <si>
+    <t>Método con 3 divisiones…</t>
+  </si>
+  <si>
+    <t>Método con 4 divisiones…</t>
+  </si>
+  <si>
+    <t>Método con 5 divisiones…</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>promedio</t>
+  </si>
+  <si>
+    <t>PRUEBA INTERESANTE… COMBINAR INTERCORR_STR_TAX con 2 divisiones (&gt;= 6 y los demás) con Prod_Freq con 3 divisiones...</t>
+  </si>
+  <si>
+    <t>[]*2</t>
+  </si>
+  <si>
+    <t>[]*3</t>
+  </si>
+  <si>
+    <t>[]*4</t>
+  </si>
+  <si>
+    <t>COMBINANDO INTERCORR_PF…. (2 divisiones)</t>
+  </si>
+  <si>
+    <t>VALE LA PENA??? O MEJOR SOLO INTERCORR_STR_TAX</t>
+  </si>
+  <si>
+    <t>PROBAR CON _NO_TAX</t>
   </si>
 </sst>
 </file>
@@ -296,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,6 +392,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,9 +404,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,19 +774,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761BBAD2-2891-4E6D-849E-CEB918A1F823}">
-  <dimension ref="B4:K27"/>
+  <dimension ref="B4:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51:O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -742,7 +795,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
@@ -751,7 +804,7 @@
         <v>0.67271899999999996</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>39</v>
       </c>
@@ -760,7 +813,7 @@
         <v>0.66870499999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -769,7 +822,7 @@
         <v>2922.2921999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -777,7 +830,7 @@
         <v>0.57750000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
@@ -788,17 +841,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
         <v>0.31719999999999998</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="4">
         <v>0.64239999999999997</v>
       </c>
@@ -808,39 +861,43 @@
       <c r="K10" s="4">
         <v>0.64319999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <f t="shared" ref="L10:L21" si="0">AVERAGE(I10:K10)</f>
+        <v>0.64149999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="14"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="4">
         <v>0.61865999999999999</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="19" t="s">
         <v>44</v>
       </c>
       <c r="G12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="4">
         <v>0.63160000000000005</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="G13" s="21" t="s">
+      <c r="D13" s="19"/>
+      <c r="G13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="18"/>
       <c r="I13" s="4">
         <v>0.65229999999999999</v>
       </c>
@@ -850,35 +907,39 @@
       <c r="K13" s="4">
         <v>0.64480000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0.65056666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="12">
         <v>0.63929999999999998</v>
       </c>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="4">
         <v>0.62629999999999997</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="4">
         <v>0.65259999999999996</v>
       </c>
@@ -888,40 +949,44 @@
       <c r="K16" s="4">
         <v>0.65739999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.65549999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="4">
         <v>0.64429999999999998</v>
       </c>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="4">
         <v>0.64558000000000004</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="20"/>
       <c r="G18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="12">
         <v>0.65820000000000001</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="G19" s="21" t="s">
+      <c r="D19" s="20"/>
+      <c r="G19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="21"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4">
         <v>0.6552</v>
       </c>
@@ -931,8 +996,12 @@
       <c r="K19" s="4">
         <v>0.66739999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>0.66020333333333336</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
@@ -946,20 +1015,26 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G22" s="21" t="s">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="21"/>
+      <c r="H22" s="18"/>
       <c r="I22" s="4">
         <v>0.66439999999999999</v>
       </c>
       <c r="J22" s="4">
         <v>0.66600000000000004</v>
       </c>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K22" s="4">
+        <v>0.66981999999999997</v>
+      </c>
+      <c r="L22" s="24">
+        <f>AVERAGE(I22:K22)</f>
+        <v>0.66674</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>46</v>
       </c>
@@ -971,7 +1046,16 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="22" t="e">
+        <f>MAX(I10,J10,K10,K13,J13,I13,I16,J16,K16,#REF!,J19,I18,I19,I21,J22,I22)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
@@ -982,7 +1066,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
@@ -991,13 +1075,179 @@
       </c>
       <c r="D27" s="16" t="s">
         <v>49</v>
+      </c>
+      <c r="G27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="K28" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="O28" s="23">
+        <v>0.66139999999999999</v>
+      </c>
+      <c r="P28">
+        <v>0.66410000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+      <c r="K29" s="25">
+        <f>AVERAGE(I30:P30)</f>
+        <v>0.67313000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="G30" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="18"/>
+      <c r="I30" s="23">
+        <v>0.6754</v>
+      </c>
+      <c r="J30" s="23">
+        <v>0.66690000000000005</v>
+      </c>
+      <c r="K30" s="23">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="L30" s="23">
+        <v>0.67279999999999995</v>
+      </c>
+      <c r="M30" s="23">
+        <v>0.67530000000000001</v>
+      </c>
+      <c r="N30" s="23">
+        <v>0.67230000000000001</v>
+      </c>
+      <c r="O30" s="23">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="P30" s="23">
+        <v>0.67183999999999999</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>0.66090000000000004</v>
+      </c>
+      <c r="J31">
+        <v>0.66239999999999999</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="J32">
+        <v>0.66210000000000002</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G34" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="18"/>
+      <c r="I34">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="36" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G37" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" s="18"/>
+      <c r="I37">
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G40" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H40" s="18"/>
+      <c r="I40">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>69</v>
+      </c>
+      <c r="J48" s="26">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="K48" s="26">
+        <v>0.67475200000000002</v>
+      </c>
+      <c r="L48" s="26">
+        <v>0.66759999999999997</v>
+      </c>
+      <c r="M48" s="26">
+        <v>0.67510000000000003</v>
+      </c>
+      <c r="N48" s="26">
+        <v>0.66359999999999997</v>
+      </c>
+      <c r="O48" s="26">
+        <v>0.67144999999999999</v>
+      </c>
+      <c r="P48" s="24">
+        <f>AVERAGE(J48:O48)</f>
+        <v>0.6709170000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N52" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:C10">
     <sortCondition descending="1" ref="C10"/>
   </sortState>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="D12:D14"/>
@@ -1029,10 +1279,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>